<commit_message>
ADD CORRECCION DE PU, REPROCESOS Y WF
</commit_message>
<xml_diff>
--- a/Ruben Chiara.xlsx
+++ b/Ruben Chiara.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="57">
   <si>
     <t># Tarea</t>
   </si>
@@ -166,13 +166,37 @@
     <t>Control de Calidad</t>
   </si>
   <si>
-    <t>Creacion de los PR para la verificacion de cantidades de registros migrados</t>
-  </si>
-  <si>
-    <t>Creacion de los PR para la verificacion de registros migrados dato a dato</t>
-  </si>
-  <si>
-    <t>Verificacion de resultados de control de calidad de datos migrados</t>
+    <t>Creacion de los PR para la verificacion de cantidades de registros migrados de Pago Unico</t>
+  </si>
+  <si>
+    <t>Creacion de los PR para la verificacion de cantidades de registros migrados de Reprocesos</t>
+  </si>
+  <si>
+    <t>Creacion de los PR para la verificacion de cantidades de registros migrados de Workflow</t>
+  </si>
+  <si>
+    <t>Creacion de los PR para la verificacion de registros migrados dato a dato de Reprocesos</t>
+  </si>
+  <si>
+    <t>Creacion de los PR para la verificacion de registros migrados dato a dato de Pago Unico</t>
+  </si>
+  <si>
+    <t>Creacion de los PR para la verificacion de registros migrados dato a dato de Workflow</t>
+  </si>
+  <si>
+    <t>Script SQL desarrollado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correr los PR de control de calidad </t>
+  </si>
+  <si>
+    <t>Revision de resultados</t>
+  </si>
+  <si>
+    <t>Verificacion del Control de Calidad</t>
+  </si>
+  <si>
+    <t>Equipo</t>
   </si>
 </sst>
 </file>
@@ -360,7 +384,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -1269,42 +1313,42 @@
     <mergeCell ref="B2:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G3">
-    <cfRule type="containsText" dxfId="22" priority="13" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="20" priority="13" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5 G7">
-    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",G5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 H7">
-    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1315,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1371,7 @@
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -1377,7 +1421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
@@ -1403,18 +1447,20 @@
         <v>42166</v>
       </c>
       <c r="I2" s="11">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="J2" s="11">
         <v>1</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+      <c r="M2" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="5">
@@ -1430,24 +1476,26 @@
         <v>27</v>
       </c>
       <c r="G3" s="8">
-        <v>42228</v>
+        <v>42223</v>
       </c>
       <c r="H3" s="8">
-        <v>42237</v>
+        <v>42166</v>
       </c>
       <c r="I3" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="11">
         <v>1</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+      <c r="M3" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="5">
@@ -1463,30 +1511,34 @@
         <v>27</v>
       </c>
       <c r="G4" s="8">
-        <v>42240</v>
+        <v>42223</v>
       </c>
       <c r="H4" s="8">
-        <v>42243</v>
+        <v>42166</v>
       </c>
       <c r="I4" s="11">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J4" s="11">
         <v>1</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="M4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="5">
         <v>4</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="E5" s="7" t="s">
         <v>38</v>
       </c>
@@ -1494,13 +1546,13 @@
         <v>27</v>
       </c>
       <c r="G5" s="8">
-        <v>42205</v>
+        <v>42228</v>
       </c>
       <c r="H5" s="8">
-        <v>42216</v>
+        <v>42237</v>
       </c>
       <c r="I5" s="11">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J5" s="11">
         <v>1</v>
@@ -1509,29 +1561,33 @@
         <v>12</v>
       </c>
       <c r="L5" s="6"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="M5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="5">
         <v>5</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="E6" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G6" s="8">
-        <v>42205</v>
+        <v>42228</v>
       </c>
       <c r="H6" s="8">
-        <v>42216</v>
+        <v>42237</v>
       </c>
       <c r="I6" s="11">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J6" s="11">
         <v>1</v>
@@ -1540,31 +1596,33 @@
         <v>12</v>
       </c>
       <c r="L6" s="6"/>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="5"/>
+      <c r="M6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="5">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="8">
-        <v>42205</v>
+        <v>42228</v>
       </c>
       <c r="H7" s="8">
-        <v>42216</v>
+        <v>42237</v>
       </c>
       <c r="I7" s="11">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J7" s="11">
         <v>1</v>
@@ -1573,63 +1631,132 @@
         <v>12</v>
       </c>
       <c r="L7" s="6"/>
-      <c r="M7" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="M7" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="5">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="8">
+        <v>42240</v>
+      </c>
+      <c r="H8" s="8">
+        <v>42243</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="5">
+        <v>8</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="8">
+        <v>42244</v>
+      </c>
+      <c r="H9" s="8">
+        <v>42247</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B6"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
-  <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="Nuevo">
+  <conditionalFormatting sqref="H2 H5">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="Nuevo">
+  <conditionalFormatting sqref="G2 G5">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Nuevo">
-      <formula>NOT(ISERROR(SEARCH("Nuevo",G5)))</formula>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Nuevo">
+      <formula>NOT(ISERROR(SEARCH("Nuevo",G9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Nuevo">
-      <formula>NOT(ISERROR(SEARCH("Nuevo",H5)))</formula>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Nuevo">
+      <formula>NOT(ISERROR(SEARCH("Nuevo",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Nuevo">
-      <formula>NOT(ISERROR(SEARCH("Nuevo",H4)))</formula>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Nuevo">
+      <formula>NOT(ISERROR(SEARCH("Nuevo",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Nuevo">
-      <formula>NOT(ISERROR(SEARCH("Nuevo",G4)))</formula>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Nuevo">
+      <formula>NOT(ISERROR(SEARCH("Nuevo",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="Nuevo">
+  <conditionalFormatting sqref="H3:H4">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Nuevo">
+      <formula>NOT(ISERROR(SEARCH("Nuevo",H3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G4">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Nuevo">
+      <formula>NOT(ISERROR(SEARCH("Nuevo",G3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:H7">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Nuevo">
+  <conditionalFormatting sqref="G6:G7">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",G6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Nuevo">
-      <formula>NOT(ISERROR(SEARCH("Nuevo",G7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Nuevo">
-      <formula>NOT(ISERROR(SEARCH("Nuevo",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2063,22 +2190,22 @@
     <mergeCell ref="B7:B11"/>
   </mergeCells>
   <conditionalFormatting sqref="H2">
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G11">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",G3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H11">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Nuevo">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Nuevo">
       <formula>NOT(ISERROR(SEARCH("Nuevo",H3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>